<commit_message>
Add video of presentation and update gitignore
- Add mp4 version of the presentation
- Update .gitignore file
</commit_message>
<xml_diff>
--- a/analysis/campaigns-analysis.xlsx
+++ b/analysis/campaigns-analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e3e6a90a7d0137c2/Desktop/ds/bcgx-campaigns-performance-analysis/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="468" documentId="13_ncr:1_{A548AC19-C501-46E1-915C-B6A7CF23C754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CE6849C-6F6E-4DDE-A9CF-A30FC31C0888}"/>
+  <xr:revisionPtr revIDLastSave="477" documentId="13_ncr:1_{A548AC19-C501-46E1-915C-B6A7CF23C754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AD38588-1500-47D5-B504-03E79BFF57C2}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" firstSheet="5" activeTab="5" xr2:uid="{0753742A-CAC4-4A7D-BFFA-893AA9730FA6}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" firstSheet="3" activeTab="3" xr2:uid="{0753742A-CAC4-4A7D-BFFA-893AA9730FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="1" r:id="rId1"/>
@@ -4932,13 +4932,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2124.4700000000003</c:v>
+                  <c:v>827.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>969.46</c:v>
+                  <c:v>1193.44</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>633.06000000000006</c:v>
+                  <c:v>121.22999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5055,13 +5055,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1382.3799999999999</c:v>
+                  <c:v>3574.5600000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>416.14</c:v>
+                  <c:v>1294.3700000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>318.92000000000007</c:v>
+                  <c:v>1803.6700000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15587,7 +15587,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{624B1E25-2610-4A59-BD61-C8757512AE04}" name="PivotTable5" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Channel">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{624B1E25-2610-4A59-BD61-C8757512AE04}" name="PivotTable5" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12" rowHeaderCaption="Channel">
   <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -15700,7 +15700,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43D82D2C-09A2-46DC-A7E5-8E5A5B84F27C}" name="PivotTable4" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19" rowHeaderCaption="Campaign Type">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43D82D2C-09A2-46DC-A7E5-8E5A5B84F27C}" name="PivotTable4" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="22" rowHeaderCaption="Campaign Type">
   <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -15791,7 +15791,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0321AFFA-6B0C-4CFC-BF51-8E9003E5E4EA}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0321AFFA-6B0C-4CFC-BF51-8E9003E5E4EA}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="17">
   <location ref="A3:D7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -15912,7 +15912,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C843F76B-5425-4CA0-927C-5EF2612B7AC3}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C843F76B-5425-4CA0-927C-5EF2612B7AC3}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13">
   <location ref="A3:D8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -15933,8 +15933,8 @@
     </pivotField>
     <pivotField showAll="0">
       <items count="3">
-        <item h="1" x="0"/>
-        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -15976,7 +15976,7 @@
   <dataFields count="1">
     <dataField name="Sum of Sales ($)" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="6">
+  <chartFormats count="2">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -15990,54 +15990,6 @@
       </pivotArea>
     </chartFormat>
     <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="8" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="8" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="5" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -16134,7 +16086,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0ACB73EA-6391-489D-82D1-7A72BBE93D50}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="49">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0ACB73EA-6391-489D-82D1-7A72BBE93D50}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="52">
   <location ref="A3:C7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -16255,8 +16207,8 @@
   <data>
     <tabular pivotCacheId="1392361296">
       <items count="2">
-        <i x="0"/>
-        <i x="1" s="1"/>
+        <i x="0" s="1"/>
+        <i x="1"/>
       </items>
     </tabular>
   </data>
@@ -28140,8 +28092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C582100-09C4-4C3C-A93B-82F85FF89FBD}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28252,8 +28204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F4AC5E-DD39-4F9A-BD56-8C561E917899}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28325,8 +28277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53715DBD-C3FC-42FF-AD67-0B2F7943C23B}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28388,8 +28340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{396F0BB9-7B0B-4982-81CE-5B17CE9AB885}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView topLeftCell="D1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28479,7 +28431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5480305F-0B7B-4EB1-AF62-723C796E65EF}">
   <dimension ref="A3:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" workbookViewId="0">
+    <sheetView zoomScale="71" workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
@@ -28518,13 +28470,13 @@
         <v>12</v>
       </c>
       <c r="B5" s="7">
-        <v>2124.4700000000003</v>
+        <v>827.9</v>
       </c>
       <c r="C5" s="7">
-        <v>1382.3799999999999</v>
+        <v>3574.5600000000004</v>
       </c>
       <c r="D5" s="7">
-        <v>3506.8500000000004</v>
+        <v>4402.46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -28532,13 +28484,13 @@
         <v>9</v>
       </c>
       <c r="B6" s="7">
-        <v>969.46</v>
+        <v>1193.44</v>
       </c>
       <c r="C6" s="7">
-        <v>416.14</v>
+        <v>1294.3700000000003</v>
       </c>
       <c r="D6" s="7">
-        <v>1385.6</v>
+        <v>2487.8100000000004</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -28546,13 +28498,13 @@
         <v>24</v>
       </c>
       <c r="B7" s="7">
-        <v>633.06000000000006</v>
+        <v>121.22999999999999</v>
       </c>
       <c r="C7" s="7">
-        <v>318.92000000000007</v>
+        <v>1803.6700000000003</v>
       </c>
       <c r="D7" s="7">
-        <v>951.98000000000013</v>
+        <v>1924.9000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -28560,13 +28512,13 @@
         <v>515</v>
       </c>
       <c r="B8" s="7">
-        <v>3726.9900000000002</v>
+        <v>2142.5700000000002</v>
       </c>
       <c r="C8" s="7">
-        <v>2117.44</v>
+        <v>6672.6</v>
       </c>
       <c r="D8" s="7">
-        <v>5844.4300000000012</v>
+        <v>8815.17</v>
       </c>
     </row>
   </sheetData>
@@ -28783,8 +28735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A24DBB-C550-4C93-A0A7-4E50ABEDF59B}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>